<commit_message>
Updated Lab Time Table
</commit_message>
<xml_diff>
--- a/3rd Year CSE, IT,CSM Timetables-1.xlsx
+++ b/3rd Year CSE, IT,CSM Timetables-1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CSE 3A" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="76">
   <si>
     <t xml:space="preserve">Aurora's Technological &amp; Research Institute</t>
   </si>
@@ -121,12 +121,21 @@
     <t xml:space="preserve">Tuesday</t>
   </si>
   <si>
+    <t xml:space="preserve">ML(B1) CD(B2)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wednesday</t>
   </si>
   <si>
+    <t xml:space="preserve">CD(B1) MAD(B2)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Thursday</t>
   </si>
   <si>
+    <t xml:space="preserve">MAD(B1) ML(B2)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Friday</t>
   </si>
   <si>
@@ -145,34 +154,133 @@
     <t xml:space="preserve">Mr. P. Venu Madhav</t>
   </si>
   <si>
+    <t xml:space="preserve">ML Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. A. Anitha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mad Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. TV Ramanamma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. S. Mahesh</t>
+  </si>
+  <si>
     <t xml:space="preserve">CLASS TIME TABLE - 2022-2023  II Semester</t>
   </si>
   <si>
     <t xml:space="preserve">CSE-III B</t>
   </si>
   <si>
+    <t xml:space="preserve">CD(B1) ML(B2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ML(B1) MAD(B2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAD(B1) CD (B2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAD Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. M. Vineela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. S. Anitha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Shilpa</t>
+  </si>
+  <si>
     <t xml:space="preserve">CSE-III C</t>
   </si>
   <si>
+    <t xml:space="preserve">MAD(B1) CD(B2)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mr. M Jagan</t>
   </si>
   <si>
     <t xml:space="preserve">CSE-III D</t>
   </si>
   <si>
+    <t xml:space="preserve">MAD LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD LAB</t>
+  </si>
+  <si>
     <t xml:space="preserve">EVS</t>
   </si>
   <si>
+    <t xml:space="preserve">ML LAB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mr. M. Jagan</t>
   </si>
   <si>
     <t xml:space="preserve">Ms. Nalini</t>
   </si>
   <si>
+    <t xml:space="preserve">Mr. AR Sofi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. V. Shilpa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Sameena</t>
+  </si>
+  <si>
     <t xml:space="preserve">IT - III</t>
   </si>
   <si>
+    <t xml:space="preserve">STM LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCC LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. M. Saravanan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCC Lab</t>
+  </si>
+  <si>
     <t xml:space="preserve">CSM-III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAD(B1) DEVOPS(B2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLP(B1)  MAD(B2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEVOPS(B1) NLP (B2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLP Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. Masood Ahmed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DevOps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Gowthami</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAD</t>
   </si>
 </sst>
 </file>
@@ -182,7 +290,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -259,6 +367,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -363,7 +476,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -448,35 +561,39 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -484,16 +601,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -575,8 +696,8 @@
   </sheetPr>
   <dimension ref="B1:N231"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -777,14 +898,16 @@
       </c>
       <c r="I11" s="14"/>
       <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
+      <c r="K11" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
       <c r="N11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="13"/>
@@ -796,14 +919,16 @@
       </c>
       <c r="I12" s="14"/>
       <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
+      <c r="K12" s="13" t="s">
+        <v>24</v>
+      </c>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
       <c r="N12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="13"/>
@@ -815,14 +940,16 @@
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
+      <c r="K13" s="13" t="s">
+        <v>26</v>
+      </c>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
       <c r="N13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="13"/>
@@ -839,7 +966,7 @@
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="13"/>
@@ -905,14 +1032,14 @@
       <c r="D19" s="8"/>
       <c r="E19" s="15"/>
       <c r="F19" s="16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="16" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
@@ -933,7 +1060,7 @@
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="20" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
@@ -949,9 +1076,13 @@
       <c r="F21" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="G21" s="19"/>
+      <c r="G21" s="19" t="s">
+        <v>33</v>
+      </c>
       <c r="H21" s="19"/>
-      <c r="I21" s="20"/>
+      <c r="I21" s="20" t="s">
+        <v>34</v>
+      </c>
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
@@ -966,9 +1097,13 @@
       <c r="F22" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="G22" s="19"/>
+      <c r="G22" s="19" t="s">
+        <v>35</v>
+      </c>
       <c r="H22" s="19"/>
-      <c r="I22" s="20"/>
+      <c r="I22" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
@@ -983,12 +1118,16 @@
       <c r="F23" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="G23" s="19"/>
+      <c r="G23" s="19" t="s">
+        <v>37</v>
+      </c>
       <c r="H23" s="19"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
+      <c r="I23" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
     </row>
@@ -1119,65 +1258,65 @@
       <c r="N31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="24" t="s">
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H32" s="24"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="21" t="s">
+      <c r="H32" s="25"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="N32" s="26"/>
+      <c r="N32" s="27"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="28"/>
-      <c r="L35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="28"/>
-      <c r="K36" s="28"/>
-      <c r="L36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1375,7 +1514,7 @@
     <row r="230" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="231" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="47">
+  <mergeCells count="50">
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B3:N3"/>
     <mergeCell ref="B5:N5"/>
@@ -1385,8 +1524,11 @@
     <mergeCell ref="I10:I15"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="K11:M11"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="K12:M12"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="K13:M13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="G19:H19"/>
@@ -1441,8 +1583,8 @@
   </sheetPr>
   <dimension ref="B1:N226"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1499,7 +1641,7 @@
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -1516,7 +1658,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1622,7 +1764,9 @@
         <v>19</v>
       </c>
       <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
+      <c r="K10" s="13" t="s">
+        <v>41</v>
+      </c>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
       <c r="N10" s="8"/>
@@ -1650,10 +1794,12 @@
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="11"/>
-      <c r="D12" s="13"/>
+      <c r="D12" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
@@ -1669,7 +1815,7 @@
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="13"/>
@@ -1688,10 +1834,12 @@
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C14" s="11"/>
-      <c r="D14" s="13"/>
+      <c r="D14" s="13" t="s">
+        <v>43</v>
+      </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -1705,7 +1853,7 @@
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="13"/>
@@ -1771,14 +1919,14 @@
       <c r="D19" s="8"/>
       <c r="E19" s="15"/>
       <c r="F19" s="16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="16" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
@@ -1799,7 +1947,7 @@
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="20" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
@@ -1815,9 +1963,13 @@
       <c r="F21" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="G21" s="19"/>
+      <c r="G21" s="19" t="s">
+        <v>44</v>
+      </c>
       <c r="H21" s="19"/>
-      <c r="I21" s="20"/>
+      <c r="I21" s="20" t="s">
+        <v>45</v>
+      </c>
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
@@ -1832,9 +1984,13 @@
       <c r="F22" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="G22" s="19"/>
+      <c r="G22" s="19" t="s">
+        <v>33</v>
+      </c>
       <c r="H22" s="19"/>
-      <c r="I22" s="20"/>
+      <c r="I22" s="20" t="s">
+        <v>46</v>
+      </c>
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
@@ -1849,9 +2005,13 @@
       <c r="F23" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="G23" s="19"/>
+      <c r="G23" s="19" t="s">
+        <v>37</v>
+      </c>
       <c r="H23" s="19"/>
-      <c r="I23" s="20"/>
+      <c r="I23" s="20" t="s">
+        <v>47</v>
+      </c>
       <c r="J23" s="20"/>
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
@@ -2180,7 +2340,7 @@
     <row r="225" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="226" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="40">
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B3:N3"/>
     <mergeCell ref="B5:N5"/>
@@ -2188,11 +2348,14 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="I10:I15"/>
+    <mergeCell ref="K10:M10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="I19:L19"/>
@@ -2236,8 +2399,8 @@
   </sheetPr>
   <dimension ref="B1:N225"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2294,7 +2457,7 @@
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -2311,7 +2474,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="5" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2404,7 +2567,9 @@
         <v>17</v>
       </c>
       <c r="C10" s="11"/>
-      <c r="D10" s="13"/>
+      <c r="D10" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
@@ -2427,7 +2592,9 @@
         <v>21</v>
       </c>
       <c r="C11" s="11"/>
-      <c r="D11" s="13"/>
+      <c r="D11" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
@@ -2443,7 +2610,7 @@
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="13"/>
@@ -2462,7 +2629,7 @@
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="13"/>
@@ -2483,7 +2650,7 @@
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="13"/>
@@ -2493,14 +2660,16 @@
       <c r="H14" s="13"/>
       <c r="I14" s="14"/>
       <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
+      <c r="K14" s="13" t="s">
+        <v>41</v>
+      </c>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
       <c r="N14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="13"/>
@@ -2566,14 +2735,14 @@
       <c r="D19" s="8"/>
       <c r="E19" s="15"/>
       <c r="F19" s="16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="16" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
@@ -2594,7 +2763,7 @@
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="20" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
@@ -2610,9 +2779,13 @@
       <c r="F21" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="G21" s="19"/>
+      <c r="G21" s="19" t="s">
+        <v>33</v>
+      </c>
       <c r="H21" s="19"/>
-      <c r="I21" s="20"/>
+      <c r="I21" s="20" t="s">
+        <v>34</v>
+      </c>
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
@@ -2627,9 +2800,13 @@
       <c r="F22" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="G22" s="19"/>
+      <c r="G22" s="19" t="s">
+        <v>44</v>
+      </c>
       <c r="H22" s="19"/>
-      <c r="I22" s="20"/>
+      <c r="I22" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
@@ -2644,9 +2821,13 @@
       <c r="F23" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="G23" s="19"/>
+      <c r="G23" s="19" t="s">
+        <v>37</v>
+      </c>
       <c r="H23" s="19"/>
-      <c r="I23" s="20"/>
+      <c r="I23" s="20" t="s">
+        <v>38</v>
+      </c>
       <c r="J23" s="20"/>
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
@@ -2974,19 +3155,22 @@
     <row r="224" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="225" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="40">
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B3:N3"/>
     <mergeCell ref="B5:N5"/>
     <mergeCell ref="B6:N6"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
     <mergeCell ref="I10:I15"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="K14:M14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="I19:L19"/>
@@ -3030,8 +3214,8 @@
   </sheetPr>
   <dimension ref="B1:N232"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3088,7 +3272,7 @@
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -3105,7 +3289,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="5" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -3209,7 +3393,9 @@
         <v>19</v>
       </c>
       <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
+      <c r="K10" s="13" t="s">
+        <v>52</v>
+      </c>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
       <c r="N10" s="8"/>
@@ -3219,11 +3405,13 @@
         <v>21</v>
       </c>
       <c r="C11" s="11"/>
-      <c r="D11" s="13"/>
+      <c r="D11" s="13" t="s">
+        <v>53</v>
+      </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>18</v>
@@ -3239,7 +3427,7 @@
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="13"/>
@@ -3250,17 +3438,19 @@
         <v>18</v>
       </c>
       <c r="I12" s="14"/>
-      <c r="J12" s="13"/>
+      <c r="J12" s="13" t="s">
+        <v>55</v>
+      </c>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="N12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="13"/>
@@ -3279,7 +3469,7 @@
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="13"/>
@@ -3288,7 +3478,7 @@
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="13" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="14"/>
@@ -3300,7 +3490,7 @@
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="13"/>
@@ -3366,14 +3556,14 @@
       <c r="D19" s="8"/>
       <c r="E19" s="15"/>
       <c r="F19" s="16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="16" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
@@ -3394,7 +3584,7 @@
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="20" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
@@ -3411,11 +3601,11 @@
         <v>2</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="20" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
@@ -3431,9 +3621,13 @@
       <c r="F22" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="G22" s="19"/>
+      <c r="G22" s="19" t="s">
+        <v>33</v>
+      </c>
       <c r="H22" s="19"/>
-      <c r="I22" s="20"/>
+      <c r="I22" s="20" t="s">
+        <v>58</v>
+      </c>
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
@@ -3448,9 +3642,13 @@
       <c r="F23" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="G23" s="19"/>
+      <c r="G23" s="19" t="s">
+        <v>37</v>
+      </c>
       <c r="H23" s="19"/>
-      <c r="I23" s="20"/>
+      <c r="I23" s="20" t="s">
+        <v>59</v>
+      </c>
       <c r="J23" s="20"/>
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
@@ -3465,9 +3663,13 @@
       <c r="F24" s="18" t="n">
         <v>5</v>
       </c>
-      <c r="G24" s="19"/>
+      <c r="G24" s="19" t="s">
+        <v>44</v>
+      </c>
       <c r="H24" s="19"/>
-      <c r="I24" s="20"/>
+      <c r="I24" s="20" t="s">
+        <v>60</v>
+      </c>
       <c r="J24" s="20"/>
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
@@ -3591,69 +3793,69 @@
       <c r="N32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="32"/>
-      <c r="N33" s="21"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="24" t="s">
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H35" s="24"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="21" t="s">
+      <c r="H35" s="25"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
+      <c r="L35" s="26"/>
+      <c r="M35" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="N35" s="26"/>
+      <c r="N35" s="27"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="28"/>
-      <c r="K36" s="28"/>
-      <c r="L36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="28"/>
-      <c r="K37" s="28"/>
-      <c r="L37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3851,7 +4053,7 @@
     <row r="231" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="232" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="47">
+  <mergeCells count="50">
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B3:N3"/>
     <mergeCell ref="B5:N5"/>
@@ -3859,9 +4061,12 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="I10:I15"/>
+    <mergeCell ref="K10:M10"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="J12:L12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
@@ -3917,8 +4122,8 @@
   </sheetPr>
   <dimension ref="B1:N232"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3977,7 +4182,7 @@
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -3994,7 +4199,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="5" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -4126,7 +4331,7 @@
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="13"/>
@@ -4138,19 +4343,23 @@
       </c>
       <c r="I12" s="14"/>
       <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
+      <c r="K12" s="13" t="s">
+        <v>62</v>
+      </c>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
       <c r="N12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" s="11"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
+      <c r="D13" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13" t="s">
         <v>18</v>
@@ -4166,7 +4375,7 @@
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="13"/>
@@ -4183,7 +4392,7 @@
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="13"/>
@@ -4249,14 +4458,14 @@
       <c r="D19" s="8"/>
       <c r="E19" s="15"/>
       <c r="F19" s="16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="16" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
@@ -4277,7 +4486,7 @@
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="20" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
@@ -4293,9 +4502,13 @@
       <c r="F21" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="G21" s="19"/>
+      <c r="G21" s="19" t="s">
+        <v>64</v>
+      </c>
       <c r="H21" s="19"/>
-      <c r="I21" s="20"/>
+      <c r="I21" s="20" t="s">
+        <v>65</v>
+      </c>
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
@@ -4310,9 +4523,13 @@
       <c r="F22" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="G22" s="19"/>
+      <c r="G22" s="19" t="s">
+        <v>66</v>
+      </c>
       <c r="H22" s="19"/>
-      <c r="I22" s="20"/>
+      <c r="I22" s="20" t="s">
+        <v>47</v>
+      </c>
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
@@ -4470,69 +4687,69 @@
       <c r="N32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="32"/>
-      <c r="N33" s="21"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="24" t="s">
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H35" s="24"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="21" t="s">
+      <c r="H35" s="25"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
+      <c r="L35" s="26"/>
+      <c r="M35" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="N35" s="26"/>
+      <c r="N35" s="27"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="28"/>
-      <c r="K36" s="28"/>
-      <c r="L36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="28"/>
-      <c r="K37" s="28"/>
-      <c r="L37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4730,7 +4947,7 @@
     <row r="231" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="232" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="47">
+  <mergeCells count="50">
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B3:N3"/>
     <mergeCell ref="B5:N5"/>
@@ -4741,7 +4958,10 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="K12:M12"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="G19:H19"/>
@@ -4796,8 +5016,8 @@
   </sheetPr>
   <dimension ref="B1:N230"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4854,7 +5074,7 @@
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -4871,7 +5091,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="5" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -4989,21 +5209,23 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="14"/>
       <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
+      <c r="K11" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
       <c r="N11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="13"/>
@@ -5020,16 +5242,18 @@
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="N12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" s="11"/>
-      <c r="D13" s="13"/>
+      <c r="D13" s="13" t="s">
+        <v>69</v>
+      </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
@@ -5038,21 +5262,23 @@
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
+      <c r="K13" s="13" t="s">
+        <v>70</v>
+      </c>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
       <c r="N13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="14"/>
@@ -5066,7 +5292,7 @@
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="13"/>
@@ -5132,14 +5358,14 @@
       <c r="D19" s="8"/>
       <c r="E19" s="15"/>
       <c r="F19" s="16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="16" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
@@ -5155,9 +5381,13 @@
       <c r="F20" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="G20" s="19"/>
+      <c r="G20" s="19" t="s">
+        <v>71</v>
+      </c>
       <c r="H20" s="19"/>
-      <c r="I20" s="20"/>
+      <c r="I20" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
@@ -5172,9 +5402,13 @@
       <c r="F21" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="G21" s="19"/>
+      <c r="G21" s="19" t="s">
+        <v>73</v>
+      </c>
       <c r="H21" s="19"/>
-      <c r="I21" s="20"/>
+      <c r="I21" s="20" t="s">
+        <v>74</v>
+      </c>
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
@@ -5189,9 +5423,13 @@
       <c r="F22" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="G22" s="19"/>
+      <c r="G22" s="19" t="s">
+        <v>75</v>
+      </c>
       <c r="H22" s="19"/>
-      <c r="I22" s="20"/>
+      <c r="I22" s="20" t="s">
+        <v>60</v>
+      </c>
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
@@ -5342,48 +5580,48 @@
       <c r="N31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="21"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="21"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="28"/>
-      <c r="L35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5581,7 +5819,7 @@
     <row r="229" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="230" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="48">
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B3:N3"/>
     <mergeCell ref="B5:N5"/>
@@ -5590,9 +5828,12 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="I10:I15"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="K11:M11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="K13:M13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="G19:H19"/>

</xml_diff>